<commit_message>
Firebase integration and marker on the Map
</commit_message>
<xml_diff>
--- a/Documents/Tableau de répartition des tâches.xlsx
+++ b/Documents/Tableau de répartition des tâches.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86440D51-635C-43D8-BF10-D9B80351F215}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DC334-2C84-4ADA-A478-3AFC11A246C9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,13 +144,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -177,19 +201,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -469,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,104 +528,104 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UI modification and load of citys Welcome screen and remove actionbar
</commit_message>
<xml_diff>
--- a/Documents/Tableau de répartition des tâches.xlsx
+++ b/Documents/Tableau de répartition des tâches.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DC334-2C84-4ADA-A478-3AFC11A246C9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB577CD-3A3C-4991-9F3E-39BAAEBA30F4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,36 +613,36 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upload picture UI and BDD
</commit_message>
<xml_diff>
--- a/Documents/Tableau de répartition des tâches.xlsx
+++ b/Documents/Tableau de répartition des tâches.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB577CD-3A3C-4991-9F3E-39BAAEBA30F4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604FC4D6-201D-463E-9E64-79C41DC18AA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,15 +151,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,11 +162,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -201,12 +189,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -214,10 +201,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -499,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,19 +615,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -732,19 +717,19 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>